<commit_message>
finish three kind devices and all of the flow
</commit_message>
<xml_diff>
--- a/documents/整体协议 .xlsx
+++ b/documents/整体协议 .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28785" windowHeight="13140"/>
+    <workbookView windowWidth="32400" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
   <si>
     <t>协议头</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>1代表固定风向，2代表左右风向</t>
+  </si>
+  <si>
+    <t>#SMARTALL,2,1,0D0H0M0S,2,1,7,5,8,2,9,15,11,1,12,0,57,*HH</t>
   </si>
   <si>
     <t>温度</t>
@@ -212,10 +215,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -235,9 +238,54 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -249,13 +297,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -264,6 +305,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -272,7 +337,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,33 +351,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,29 +362,6 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -353,22 +372,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -391,19 +394,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,73 +556,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,79 +568,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,17 +597,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -626,11 +623,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -640,6 +635,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,166 +671,159 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -835,87 +838,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="23" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="23" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="23" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="58" fontId="1" fillId="3" borderId="1" xfId="26" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="1" fillId="3" borderId="1" xfId="23" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="23" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1182,15 +1185,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:K15"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4"/>
   <cols>
     <col min="1" max="1" width="29.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
@@ -1240,7 +1243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="15" spans="1:11">
+    <row r="2" ht="13.15" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:14">
+    <row r="3" ht="14.25" customHeight="1" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1282,7 +1285,7 @@
       </c>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" ht="15.75" spans="1:14">
+    <row r="4" ht="14.5" spans="1:14">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1301,7 +1304,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:14">
+    <row r="5" ht="13.9" spans="1:14">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1320,7 +1323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:14">
+    <row r="6" ht="13.9" spans="1:14">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1339,7 +1342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:11">
+    <row r="7" ht="13.9" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1354,7 +1357,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" ht="15.75" spans="1:14">
+    <row r="8" ht="13.9" spans="1:14">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1371,7 +1374,7 @@
       </c>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" ht="15.75" spans="1:14">
+    <row r="9" ht="14.5" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,16 +1387,16 @@
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1412,15 +1415,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="1:14">
-      <c r="A10" s="5" t="s">
+    <row r="10" ht="14.5" spans="1:14">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="6"/>
@@ -1431,11 +1434,11 @@
       <c r="H10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M10" s="9" t="s">
@@ -1445,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="15.75" spans="1:14">
+    <row r="11" ht="13.9" spans="1:14">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:14">
+    <row r="12" ht="13.9" spans="1:14">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1485,7 +1488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:11">
+    <row r="13" ht="13.9" spans="1:11">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1498,7 +1501,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" ht="13.9" spans="1:18">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1521,8 +1524,8 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" ht="15.75" spans="1:18">
-      <c r="A15" s="5"/>
+    <row r="15" ht="13.9" spans="1:18">
+      <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1554,18 +1557,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="1:18">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+    <row r="16" ht="13.9" spans="1:18">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
       <c r="M16" s="9" t="s">
         <v>31</v>
       </c>
@@ -1585,18 +1588,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="1:18">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+    <row r="17" ht="13.9" spans="1:18">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
       <c r="M17" s="9" t="s">
         <v>36</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="13:18">
+    <row r="18" ht="13.9" spans="13:18">
       <c r="M18" s="9" t="s">
         <v>39</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="13:18">
+    <row r="19" ht="13.9" spans="13:18">
       <c r="M19" s="9" t="s">
         <v>41</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="13:18">
+    <row r="20" ht="13.9" spans="13:18">
       <c r="M20" s="9" t="s">
         <v>42</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="13:18">
+    <row r="21" ht="13.9" spans="13:18">
       <c r="M21" s="9" t="s">
         <v>44</v>
       </c>
@@ -1692,7 +1695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="13:18">
+    <row r="22" ht="13.9" spans="13:18">
       <c r="M22" s="9" t="s">
         <v>45</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" ht="15.75" spans="13:18">
+    <row r="23" ht="13.9" spans="13:18">
       <c r="M23" s="9" t="s">
         <v>48</v>
       </c>
@@ -1732,9 +1735,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="13:18">
+    <row r="24" ht="13.9" spans="5:18">
+      <c r="E24" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="M24" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N24" s="9">
         <v>9</v>
@@ -1743,7 +1749,7 @@
         <v>50</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q24" s="9" t="s">
         <v>34</v>
@@ -1752,9 +1758,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" ht="15.75" spans="13:18">
+    <row r="25" ht="13.9" spans="13:18">
       <c r="M25" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N25" s="9">
         <v>10</v>
@@ -1763,7 +1769,7 @@
         <v>37</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q25" s="9" t="s">
         <v>34</v>
@@ -1772,9 +1778,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="13:18">
+    <row r="26" ht="13.9" spans="13:18">
       <c r="M26" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N26" s="9">
         <v>11</v>
@@ -1783,7 +1789,7 @@
         <v>37</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q26" s="9" t="s">
         <v>34</v>
@@ -1792,9 +1798,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="13:18">
+    <row r="27" ht="13.9" spans="13:18">
       <c r="M27" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N27" s="9">
         <v>12</v>
@@ -1803,7 +1809,7 @@
         <v>37</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>34</v>
@@ -1812,9 +1818,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="13:18">
+    <row r="28" ht="13.9" spans="13:18">
       <c r="M28" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N28" s="9">
         <v>13</v>
@@ -1823,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q28" s="9" t="s">
         <v>35</v>
@@ -1832,9 +1838,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" ht="15.75" spans="13:18">
+    <row r="29" ht="13.9" spans="13:18">
       <c r="M29" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N29" s="9">
         <v>14</v>
@@ -1843,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q29" s="9" t="s">
         <v>35</v>
@@ -1852,9 +1858,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" ht="15.75" spans="13:18">
+    <row r="30" ht="13.9" spans="13:18">
       <c r="M30" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
@@ -1862,7 +1868,7 @@
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
     </row>
-    <row r="31" spans="13:18">
+    <row r="31" ht="13.9" spans="13:18">
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -1870,7 +1876,7 @@
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
     </row>
-    <row r="32" ht="15"/>
+    <row r="32" ht="13.15"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="M3:N3"/>
@@ -1886,7 +1892,7 @@
     <mergeCell ref="A11:K13"/>
     <mergeCell ref="M30:R31"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>

</xml_diff>